<commit_message>
Finished running all NCDE classifications
</commit_message>
<xml_diff>
--- a/Results/Classification/Control vs Atypical/Classification Summary.xlsx
+++ b/Results/Classification/Control vs Atypical/Classification Summary.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopher/Documents/PTSD/NCDE Model.nosync/Results/Classification/Control vs Atypical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D97D7CE-C14E-AA4A-AC9A-1830C4F73B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C063CAA3-A87F-1248-AEB6-81ADF0B07C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{062D004C-F53A-1D47-97C0-0B8F3220FE90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Control</t>
   </si>
   <si>
     <t>Atypical</t>
+  </si>
+  <si>
+    <t>100 Iterations</t>
   </si>
 </sst>
 </file>
@@ -77,13 +80,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -107,13 +109,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -453,144 +455,302 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99621FD6-3A7B-D04E-89EF-35E6FCECDE0F}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E2" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <f>SUM(C3:E3)/30</f>
-        <v>0.6</v>
-      </c>
-      <c r="H3">
-        <v>0.5</v>
-      </c>
-      <c r="I3">
-        <v>0.7</v>
-      </c>
-      <c r="J3">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="2"/>
       <c r="C4">
         <v>5</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F4">
         <f>SUM(C4:E4)/30</f>
-        <v>0.43333333333333335</v>
+        <v>0.5</v>
       </c>
       <c r="H4">
+        <f>C4/10</f>
         <v>0.5</v>
       </c>
       <c r="I4">
-        <v>0.6</v>
+        <f t="shared" ref="I4:J4" si="0">D4/10</f>
+        <v>0.5</v>
       </c>
       <c r="J4">
-        <v>0.2</v>
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <f>SUM(C5:E5)/30</f>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="H5">
+        <f>C5/10</f>
+        <v>0.7</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5" si="1">D5/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5" si="2">E5/10</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5">
+      <c r="B6" s="2"/>
+      <c r="C6">
         <v>4</v>
       </c>
-      <c r="F5">
-        <f>SUM(C5:E5)/27</f>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <f>SUM(C6:E6)/27</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="H6" s="1">
+        <f>C6/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" ref="I6:J6" si="3">D6/9</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="H5" s="3">
+      <c r="J6" s="1">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f>SUM(C4:C6)/29</f>
+        <v>0.55172413793103448</v>
+      </c>
+      <c r="D7">
+        <f>SUM(D4:D6)/29</f>
+        <v>0.51724137931034486</v>
+      </c>
+      <c r="E7">
+        <f>SUM(E4:E6)/29</f>
+        <v>0.44827586206896552</v>
+      </c>
+      <c r="F7">
+        <f>SUM(C4:E6)/87</f>
+        <v>0.50574712643678166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <f>SUM(C11:E11)/30</f>
+        <v>0.5</v>
+      </c>
+      <c r="H11">
+        <f>C11/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11:I12" si="4">D11/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ref="J11:J12" si="5">E11/10</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <f>SUM(C12:E12)/30</f>
+        <v>0.5</v>
+      </c>
+      <c r="H12">
+        <f>C12/10</f>
+        <v>0.7</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="5"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <f>SUM(C13:E13)/27</f>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="H13">
+        <f>C13/9</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="I5">
-        <v>0.67</v>
-      </c>
-      <c r="J5">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C6">
-        <f>SUM(C3:C5)/29</f>
-        <v>0.51724137931034486</v>
-      </c>
-      <c r="D6">
-        <f>SUM(D3:D5)/29</f>
-        <v>0.65517241379310343</v>
-      </c>
-      <c r="E6">
-        <f>SUM(E3:E5)/29</f>
-        <v>0.41379310344827586</v>
-      </c>
-      <c r="F6">
-        <f>SUM(C3:E5)/87</f>
-        <v>0.52873563218390807</v>
+      <c r="I13">
+        <f t="shared" ref="I13" si="6">D13/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ref="J13" si="7">E13/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <f>SUM(C11:C13)/29</f>
+        <v>0.58620689655172409</v>
+      </c>
+      <c r="D14">
+        <f>SUM(D11:D13)/29</f>
+        <v>0.48275862068965519</v>
+      </c>
+      <c r="E14">
+        <f>SUM(E11:E13)/29</f>
+        <v>0.34482758620689657</v>
+      </c>
+      <c r="F14">
+        <f>SUM(C11:E13)/87</f>
+        <v>0.47126436781609193</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A3:B3"/>
+  <mergeCells count="12">
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
   </mergeCells>

</xml_diff>

<commit_message>
Should be just about done editing this
</commit_message>
<xml_diff>
--- a/Results/Classification/Control vs Atypical/Classification Summary.xlsx
+++ b/Results/Classification/Control vs Atypical/Classification Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopher/Documents/PTSD/NCDE Model.nosync/Results/Classification/Control vs Atypical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A25D40-620D-774F-A271-430678796DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3382E060-A2B5-9943-B7FD-23E8EF087A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16620" xr2:uid="{062D004C-F53A-1D47-97C0-0B8F3220FE90}"/>
+    <workbookView xWindow="10360" yWindow="1180" windowWidth="28040" windowHeight="16620" xr2:uid="{062D004C-F53A-1D47-97C0-0B8F3220FE90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
   <si>
     <t>Control</t>
   </si>
@@ -52,14 +52,31 @@
   <si>
     <t>NODE</t>
   </si>
+  <si>
+    <t>ANN</t>
+  </si>
+  <si>
+    <t>200 Iterations</t>
+  </si>
+  <si>
+    <t>RNN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -86,12 +103,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,6 +206,106 @@
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
           <a:off x="0" y="431800"/>
+          <a:ext cx="1651000" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AE764F5-1AB2-2344-A6C8-E544D5332105}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="0" y="3810000"/>
+          <a:ext cx="1651000" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{523B3929-1E63-EF4A-94BD-4AD619C617FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="0" y="7124700"/>
           <a:ext cx="1651000" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -511,16 +629,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99621FD6-3A7B-D04E-89EF-35E6FCECDE0F}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -664,7 +782,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -800,8 +918,8 @@
         <v>0.47126436781609193</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -837,21 +955,30 @@
         <v>0</v>
       </c>
       <c r="B21" s="2"/>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
       <c r="F21">
         <f>SUM(C21:E21)/30</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H21">
         <f>C21/10</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I21">
         <f t="shared" ref="I21:I22" si="8">D21/10</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J21">
         <f t="shared" ref="J21:J22" si="9">E21/10</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -859,21 +986,30 @@
         <v>1</v>
       </c>
       <c r="B22" s="2"/>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
       <c r="F22">
         <f>SUM(C22:E22)/30</f>
-        <v>0</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="H22">
         <f>C22/10</f>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I22">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J22">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -881,44 +1017,53 @@
         <v>2</v>
       </c>
       <c r="B23" s="2"/>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
       <c r="F23">
         <f>SUM(C23:E23)/27</f>
-        <v>0</v>
+        <v>0.48148148148148145</v>
       </c>
       <c r="H23" s="1">
         <f>C23/9</f>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" ref="I23" si="10">D23/9</f>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" ref="J23" si="11">E23/9</f>
-        <v>0</v>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C24">
         <f>SUM(C21:C23)/29</f>
-        <v>0</v>
+        <v>0.41379310344827586</v>
       </c>
       <c r="D24">
         <f>SUM(D21:D23)/29</f>
-        <v>0</v>
+        <v>0.48275862068965519</v>
       </c>
       <c r="E24">
         <f>SUM(E21:E23)/29</f>
-        <v>0</v>
+        <v>0.62068965517241381</v>
       </c>
       <c r="F24">
         <f>SUM(C21:E23)/87</f>
-        <v>0</v>
+        <v>0.50574712643678166</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -948,21 +1093,30 @@
         <v>0</v>
       </c>
       <c r="B28" s="2"/>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
       <c r="F28">
         <f>SUM(C28:E28)/30</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H28">
         <f>C28/10</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I28">
         <f t="shared" ref="I28:I29" si="12">D28/10</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J28">
         <f t="shared" ref="J28:J29" si="13">E28/10</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -970,21 +1124,30 @@
         <v>1</v>
       </c>
       <c r="B29" s="2"/>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>8</v>
+      </c>
       <c r="F29">
         <f>SUM(C29:E29)/30</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H29">
         <f>C29/10</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I29">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J29">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -992,43 +1155,638 @@
         <v>2</v>
       </c>
       <c r="B30" s="2"/>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
       <c r="F30">
         <f>SUM(C30:E30)/27</f>
-        <v>0</v>
+        <v>0.48148148148148145</v>
       </c>
       <c r="H30">
         <f>C30/9</f>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="I30">
         <f t="shared" ref="I30" si="14">D30/9</f>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="J30">
         <f t="shared" ref="J30" si="15">E30/9</f>
-        <v>0</v>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C31">
         <f>SUM(C28:C30)/29</f>
-        <v>0</v>
+        <v>0.37931034482758619</v>
       </c>
       <c r="D31">
         <f>SUM(D28:D30)/29</f>
-        <v>0</v>
+        <v>0.48275862068965519</v>
       </c>
       <c r="E31">
         <f>SUM(E28:E30)/29</f>
-        <v>0</v>
+        <v>0.62068965517241381</v>
       </c>
       <c r="F31">
         <f>SUM(C28:E30)/87</f>
-        <v>0</v>
+        <v>0.4942528735632184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>6</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <f>SUM(C37:E37)/30</f>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="H37">
+        <f>C37/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="I37">
+        <f t="shared" ref="I37:I38" si="16">D37/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="J37">
+        <f t="shared" ref="J37:J38" si="17">E37/10</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <f>SUM(C38:E38)/30</f>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="H38">
+        <f>C38/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="16"/>
+        <v>0.4</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="17"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>2</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <f>SUM(C39:E39)/27</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="H39" s="1">
+        <f>C39/9</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" ref="I39" si="18">D39/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J39" s="1">
+        <f t="shared" ref="J39" si="19">E39/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <f>SUM(C37:C39)/29</f>
+        <v>0.62068965517241381</v>
+      </c>
+      <c r="D40">
+        <f>SUM(D37:D39)/29</f>
+        <v>0.48275862068965519</v>
+      </c>
+      <c r="E40">
+        <f>SUM(E37:E39)/29</f>
+        <v>0.41379310344827586</v>
+      </c>
+      <c r="F40">
+        <f>SUM(C37:E39)/87</f>
+        <v>0.50574712643678166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>0</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>6</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <f>SUM(C44:E44)/30</f>
+        <v>0.5</v>
+      </c>
+      <c r="H44">
+        <f>C44/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="I44">
+        <f t="shared" ref="I44:I45" si="20">D44/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="J44">
+        <f t="shared" ref="J44:J45" si="21">E44/10</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <f>SUM(C45:E45)/30</f>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="H45">
+        <f>C45/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="20"/>
+        <v>0.4</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="21"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>2</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <f>SUM(C46:E46)/27</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="H46">
+        <f>C46/9</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="I46">
+        <f t="shared" ref="I46" si="22">D46/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J46">
+        <f t="shared" ref="J46" si="23">E46/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <f>SUM(C44:C46)/29</f>
+        <v>0.62068965517241381</v>
+      </c>
+      <c r="D47">
+        <f>SUM(D44:D46)/29</f>
+        <v>0.48275862068965519</v>
+      </c>
+      <c r="E47">
+        <f>SUM(E44:E46)/29</f>
+        <v>0.37931034482758619</v>
+      </c>
+      <c r="F47">
+        <f>SUM(C44:E46)/87</f>
+        <v>0.4942528735632184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>0</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>6</v>
+      </c>
+      <c r="E53">
+        <v>7</v>
+      </c>
+      <c r="F53">
+        <f>SUM(C53:E53)/30</f>
+        <v>0.6</v>
+      </c>
+      <c r="H53">
+        <f>C53/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="I53">
+        <f t="shared" ref="I53:I54" si="24">D53/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="J53">
+        <f t="shared" ref="J53:J54" si="25">E53/10</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>1</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>7</v>
+      </c>
+      <c r="E54">
+        <v>5</v>
+      </c>
+      <c r="F54">
+        <f>SUM(C54:E54)/30</f>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="H54">
+        <f>C54/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="24"/>
+        <v>0.7</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="25"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>2</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <v>6</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
+      <c r="F55">
+        <f>SUM(C55:E55)/27</f>
+        <v>0.62962962962962965</v>
+      </c>
+      <c r="H55" s="1">
+        <f>C55/9</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="I55" s="1">
+        <f t="shared" ref="I55" si="26">D55/9</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J55" s="1">
+        <f t="shared" ref="J55" si="27">E55/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <f>SUM(C53:C55)/29</f>
+        <v>0.55172413793103448</v>
+      </c>
+      <c r="D56">
+        <f>SUM(D53:D55)/29</f>
+        <v>0.65517241379310343</v>
+      </c>
+      <c r="E56">
+        <f>SUM(E53:E55)/29</f>
+        <v>0.55172413793103448</v>
+      </c>
+      <c r="F56">
+        <f>SUM(C53:E55)/87</f>
+        <v>0.58620689655172409</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1</v>
+      </c>
+      <c r="E58" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>0</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60">
+        <v>6</v>
+      </c>
+      <c r="D60">
+        <v>6</v>
+      </c>
+      <c r="E60">
+        <v>7</v>
+      </c>
+      <c r="F60">
+        <f>SUM(C60:E60)/30</f>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="H60">
+        <f>C60/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="I60">
+        <f t="shared" ref="I60:I61" si="28">D60/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="J60">
+        <f t="shared" ref="J60:J61" si="29">E60/10</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>1</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61">
+        <v>7</v>
+      </c>
+      <c r="E61">
+        <v>5</v>
+      </c>
+      <c r="F61">
+        <f>SUM(C61:E61)/30</f>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="H61">
+        <f>C61/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="28"/>
+        <v>0.7</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="29"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>2</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62">
+        <v>6</v>
+      </c>
+      <c r="D62">
+        <v>5</v>
+      </c>
+      <c r="E62">
+        <v>4</v>
+      </c>
+      <c r="F62">
+        <f>SUM(C62:E62)/27</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="H62">
+        <f>C62/9</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I62">
+        <f t="shared" ref="I62" si="30">D62/9</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="J62">
+        <f t="shared" ref="J62" si="31">E62/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C63">
+        <f>SUM(C60:C62)/29</f>
+        <v>0.55172413793103448</v>
+      </c>
+      <c r="D63">
+        <f>SUM(D60:D62)/29</f>
+        <v>0.62068965517241381</v>
+      </c>
+      <c r="E63">
+        <f>SUM(E60:E62)/29</f>
+        <v>0.55172413793103448</v>
+      </c>
+      <c r="F63">
+        <f>SUM(C60:E62)/87</f>
+        <v>0.57471264367816088</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="48">
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A23:B23"/>

</xml_diff>